<commit_message>
update documentation of upload form.
</commit_message>
<xml_diff>
--- a/rotmic/static/uploadexample_dnacomponent.xlsx
+++ b/rotmic/static/uploadexample_dnacomponent.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="43">
   <si>
     <t>ID</t>
   </si>
@@ -143,9 +143,6 @@
   </si>
   <si>
     <t>AmpR, KanR</t>
-  </si>
-  <si>
-    <t>Clear the example data (except Status and Type columns) before inserting your own data.</t>
   </si>
   <si>
     <t>This is an example vector backbone. Multiple markers can be specified by name or ID, separated by comma.</t>
@@ -232,6 +229,92 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9525" y="219075"/>
+          <a:ext cx="10601325" cy="485775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>* Clear the example data (except Status and Type columns) before inserting your own data!</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>* Markers can be referenced by their ID or by their Name (but by ID is safer). You do NOT</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> need to specify markers for plasmid constructs -- markers will be taken from the associated Vector Backbnone.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>* If left empty, the new construct's name will be automatically composed from insert and vector names (only for plasmid entries).</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -519,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -540,128 +623,99 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
+    <row r="7" spans="1:9">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="30">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -920,17 +974,42 @@
         <v>10</v>
       </c>
     </row>
+    <row r="43" spans="3:4">
+      <c r="C43" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="3:4">
+      <c r="C44" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="3:4">
+      <c r="C45" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C42">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C45">
       <formula1>statusChoices</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D42">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:D45">
       <formula1>typeChoices</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="2400" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
include fragment / CDS as available type
</commit_message>
<xml_diff>
--- a/rotmic/static/uploadexample_dnacomponent.xlsx
+++ b/rotmic/static/uploadexample_dnacomponent.xlsx
@@ -12,7 +12,7 @@
   </sheets>
   <definedNames>
     <definedName name="statusChoices">predefined!$A$5:$A$8</definedName>
-    <definedName name="typeChoices">predefined!$C$5:$C$16</definedName>
+    <definedName name="typeChoices">predefined!$C$5:$C$17</definedName>
     <definedName name="validStatus">predefined!$A$5:$A$8</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="44">
   <si>
     <t>ID</t>
   </si>
@@ -150,6 +150,9 @@
   <si>
     <t>mTq2 expression plasmid_x000D_
 _x000D_test construct (hypothetical)</t>
+  </si>
+  <si>
+    <t>Fragment / CDS</t>
   </si>
 </sst>
 </file>
@@ -605,7 +608,7 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -723,7 +726,7 @@
         <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1018,7 +1021,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1066,7 +1069,7 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="L6" t="s">
         <v>24</v>
@@ -1077,7 +1080,7 @@
         <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L7" t="s">
         <v>24</v>
@@ -1088,7 +1091,7 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L8" t="s">
         <v>24</v>
@@ -1096,7 +1099,7 @@
     </row>
     <row r="9" spans="1:12">
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L9" t="s">
         <v>24</v>
@@ -1104,7 +1107,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="C10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L10" t="s">
         <v>24</v>
@@ -1112,7 +1115,7 @@
     </row>
     <row r="11" spans="1:12">
       <c r="C11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L11" t="s">
         <v>24</v>
@@ -1120,7 +1123,7 @@
     </row>
     <row r="12" spans="1:12">
       <c r="C12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L12" t="s">
         <v>24</v>
@@ -1128,7 +1131,7 @@
     </row>
     <row r="13" spans="1:12">
       <c r="C13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L13" t="s">
         <v>24</v>
@@ -1136,7 +1139,7 @@
     </row>
     <row r="14" spans="1:12">
       <c r="C14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L14" t="s">
         <v>24</v>
@@ -1144,7 +1147,7 @@
     </row>
     <row r="15" spans="1:12">
       <c r="C15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L15" t="s">
         <v>24</v>
@@ -1152,18 +1155,21 @@
     </row>
     <row r="16" spans="1:12">
       <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="L16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12">
+      <c r="C17" t="s">
         <v>36</v>
       </c>
-      <c r="L16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="12:12">
       <c r="L17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="12:12">
+    <row r="18" spans="3:12">
       <c r="L18" t="s">
         <v>24</v>
       </c>

</xml_diff>